<commit_message>
working (except ozon & wildberries)
</commit_message>
<xml_diff>
--- a/doc/template/mtov_ip.xlsx
+++ b/doc/template/mtov_ip.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
   <si>
     <t>№</t>
   </si>
@@ -118,12 +118,6 @@
   </si>
   <si>
     <t>Единый бесплатный телефон: 8 (800) 200-26-78</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Товарный чек № ИП-{num} от </t>
-  </si>
-  <si>
-    <t>Продавец: ИП Кокшаров Александр Сергеевич</t>
   </si>
   <si>
     <r>
@@ -209,9 +203,6 @@
     </r>
   </si>
   <si>
-    <t>ИП Кокшаров Александрр Сергеевич</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -464,6 +455,12 @@
   <si>
     <t>[*vendor*]</t>
   </si>
+  <si>
+    <t>Продавец: Музмарт</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Товарный чек № КИП-{num} от </t>
+  </si>
 </sst>
 </file>
 
@@ -793,7 +790,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -958,11 +955,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1140,138 +1176,140 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1284,83 +1322,72 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1370,6 +1397,45 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1399,7 +1465,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>211117</xdr:colOff>
+      <xdr:colOff>280390</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>693190</xdr:rowOff>
     </xdr:to>
@@ -1824,14 +1890,14 @@
   </sheetPr>
   <dimension ref="B1:AF93"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="55" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="U51" sqref="C1:V51"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="40" zoomScaleNormal="85" zoomScaleSheetLayoutView="40" workbookViewId="0">
+      <selection activeCell="U49" sqref="A1:V49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="29.5" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="2.54296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="0.6328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="0.1796875" style="1" customWidth="1"/>
     <col min="3" max="3" width="7.453125" style="1" customWidth="1"/>
     <col min="4" max="4" width="3.90625" style="1" customWidth="1"/>
     <col min="5" max="5" width="28.26953125" style="1" customWidth="1"/>
@@ -1840,7 +1906,7 @@
     <col min="8" max="8" width="19.1796875" style="1" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="9.81640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="8.08984375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.81640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.81640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="3.26953125" style="1" customWidth="1"/>
     <col min="13" max="13" width="5.7265625" style="1" customWidth="1"/>
     <col min="14" max="14" width="1.7265625" style="1" customWidth="1"/>
@@ -1850,8 +1916,8 @@
     <col min="18" max="18" width="2.7265625" style="1" customWidth="1"/>
     <col min="19" max="19" width="1.7265625" style="1" customWidth="1"/>
     <col min="20" max="20" width="0.453125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="2.1796875" style="1" customWidth="1"/>
-    <col min="22" max="22" width="0.54296875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="4.81640625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="0.26953125" style="1" customWidth="1"/>
     <col min="23" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
@@ -1860,69 +1926,67 @@
     <row r="4" spans="3:21" ht="13" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="5" spans="3:21" ht="61" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="6" spans="3:21" ht="35" x14ac:dyDescent="0.55000000000000004">
-      <c r="C6" s="100" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="100"/>
-      <c r="H6" s="100"/>
-      <c r="I6" s="100"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="100"/>
-      <c r="M6" s="100"/>
-      <c r="N6" s="100"/>
-      <c r="O6" s="100"/>
-      <c r="P6" s="100"/>
-      <c r="Q6" s="100"/>
-      <c r="R6" s="100"/>
-      <c r="S6" s="100"/>
-      <c r="T6" s="100"/>
-      <c r="U6" s="100"/>
+      <c r="C6" s="121"/>
+      <c r="D6" s="121"/>
+      <c r="E6" s="121"/>
+      <c r="F6" s="121"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="121"/>
+      <c r="I6" s="121"/>
+      <c r="J6" s="121"/>
+      <c r="K6" s="121"/>
+      <c r="L6" s="121"/>
+      <c r="M6" s="121"/>
+      <c r="N6" s="121"/>
+      <c r="O6" s="121"/>
+      <c r="P6" s="121"/>
+      <c r="Q6" s="121"/>
+      <c r="R6" s="121"/>
+      <c r="S6" s="121"/>
+      <c r="T6" s="121"/>
+      <c r="U6" s="121"/>
     </row>
     <row r="7" spans="3:21" ht="54" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C7" s="111" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="111"/>
-      <c r="E7" s="111"/>
-      <c r="F7" s="111"/>
-      <c r="G7" s="111"/>
-      <c r="H7" s="111"/>
-      <c r="I7" s="111"/>
-      <c r="J7" s="111"/>
-      <c r="K7" s="111"/>
-      <c r="L7" s="111"/>
-      <c r="M7" s="111"/>
-      <c r="N7" s="111"/>
-      <c r="O7" s="111"/>
-      <c r="P7" s="111"/>
-      <c r="Q7" s="111"/>
-      <c r="R7" s="111"/>
-      <c r="S7" s="111"/>
-      <c r="T7" s="111"/>
-      <c r="U7" s="111"/>
+      <c r="C7" s="131" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="131"/>
+      <c r="E7" s="131"/>
+      <c r="F7" s="131"/>
+      <c r="G7" s="131"/>
+      <c r="H7" s="131"/>
+      <c r="I7" s="131"/>
+      <c r="J7" s="131"/>
+      <c r="K7" s="131"/>
+      <c r="L7" s="131"/>
+      <c r="M7" s="131"/>
+      <c r="N7" s="131"/>
+      <c r="O7" s="131"/>
+      <c r="P7" s="131"/>
+      <c r="Q7" s="131"/>
+      <c r="R7" s="131"/>
+      <c r="S7" s="131"/>
+      <c r="T7" s="131"/>
+      <c r="U7" s="131"/>
     </row>
     <row r="8" spans="3:21" ht="30.5" x14ac:dyDescent="0.6">
-      <c r="C8" s="108" t="s">
+      <c r="C8" s="128" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="108"/>
-      <c r="E8" s="108"/>
-      <c r="F8" s="108"/>
-      <c r="G8" s="108"/>
-      <c r="H8" s="108"/>
-      <c r="I8" s="108"/>
-      <c r="J8" s="108"/>
-      <c r="K8" s="108"/>
-      <c r="L8" s="108"/>
-      <c r="M8" s="108"/>
-      <c r="N8" s="108"/>
-      <c r="O8" s="108"/>
-      <c r="P8" s="108"/>
-      <c r="Q8" s="108"/>
+      <c r="D8" s="128"/>
+      <c r="E8" s="128"/>
+      <c r="F8" s="128"/>
+      <c r="G8" s="128"/>
+      <c r="H8" s="128"/>
+      <c r="I8" s="128"/>
+      <c r="J8" s="128"/>
+      <c r="K8" s="128"/>
+      <c r="L8" s="128"/>
+      <c r="M8" s="128"/>
+      <c r="N8" s="128"/>
+      <c r="O8" s="128"/>
+      <c r="P8" s="128"/>
+      <c r="Q8" s="128"/>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
@@ -1972,16 +2036,16 @@
     </row>
     <row r="11" spans="3:21" ht="30" x14ac:dyDescent="0.55000000000000004">
       <c r="C11" s="4" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="K11" s="109" t="s">
+      <c r="K11" s="129" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="109"/>
-      <c r="M11" s="109"/>
-      <c r="N11" s="109"/>
+      <c r="L11" s="129"/>
+      <c r="M11" s="129"/>
+      <c r="N11" s="129"/>
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
@@ -2032,63 +2096,63 @@
       <c r="C14" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="133" t="s">
+      <c r="D14" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="133"/>
-      <c r="F14" s="133"/>
-      <c r="G14" s="133"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
       <c r="H14" s="43"/>
-      <c r="I14" s="113" t="s">
+      <c r="I14" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="J14" s="114"/>
-      <c r="K14" s="113" t="s">
+      <c r="J14" s="92"/>
+      <c r="K14" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="L14" s="137"/>
-      <c r="M14" s="114"/>
-      <c r="N14" s="113" t="s">
+      <c r="L14" s="91"/>
+      <c r="M14" s="92"/>
+      <c r="N14" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="O14" s="137"/>
-      <c r="P14" s="137"/>
-      <c r="Q14" s="137"/>
-      <c r="R14" s="137"/>
-      <c r="S14" s="137"/>
-      <c r="T14" s="137"/>
-      <c r="U14" s="114"/>
+      <c r="O14" s="91"/>
+      <c r="P14" s="91"/>
+      <c r="Q14" s="91"/>
+      <c r="R14" s="91"/>
+      <c r="S14" s="91"/>
+      <c r="T14" s="91"/>
+      <c r="U14" s="92"/>
     </row>
     <row r="15" spans="3:21" ht="86.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C15" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="134" t="s">
+      <c r="D15" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="135"/>
-      <c r="F15" s="135"/>
-      <c r="G15" s="135"/>
+      <c r="E15" s="88"/>
+      <c r="F15" s="88"/>
+      <c r="G15" s="88"/>
       <c r="H15" s="44"/>
-      <c r="I15" s="115" t="s">
+      <c r="I15" s="134" t="s">
         <v>8</v>
       </c>
-      <c r="J15" s="115"/>
-      <c r="K15" s="104" t="s">
+      <c r="J15" s="134"/>
+      <c r="K15" s="124" t="s">
         <v>9</v>
       </c>
-      <c r="L15" s="105"/>
-      <c r="M15" s="106"/>
-      <c r="N15" s="104" t="s">
+      <c r="L15" s="125"/>
+      <c r="M15" s="126"/>
+      <c r="N15" s="124" t="s">
         <v>10</v>
       </c>
-      <c r="O15" s="105"/>
-      <c r="P15" s="105"/>
-      <c r="Q15" s="105"/>
-      <c r="R15" s="105"/>
-      <c r="S15" s="105"/>
-      <c r="T15" s="105"/>
-      <c r="U15" s="106"/>
+      <c r="O15" s="125"/>
+      <c r="P15" s="125"/>
+      <c r="Q15" s="125"/>
+      <c r="R15" s="125"/>
+      <c r="S15" s="125"/>
+      <c r="T15" s="125"/>
+      <c r="U15" s="126"/>
     </row>
     <row r="16" spans="3:21" ht="5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C16" s="6"/>
@@ -2121,41 +2185,41 @@
       <c r="I17" s="9"/>
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
-      <c r="L17" s="110"/>
-      <c r="M17" s="110"/>
-      <c r="N17" s="110"/>
-      <c r="O17" s="110"/>
-      <c r="P17" s="112"/>
-      <c r="Q17" s="112"/>
-      <c r="R17" s="112"/>
-      <c r="S17" s="112"/>
-      <c r="T17" s="112"/>
-      <c r="U17" s="112"/>
+      <c r="L17" s="130"/>
+      <c r="M17" s="130"/>
+      <c r="N17" s="130"/>
+      <c r="O17" s="130"/>
+      <c r="P17" s="132"/>
+      <c r="Q17" s="132"/>
+      <c r="R17" s="132"/>
+      <c r="S17" s="132"/>
+      <c r="T17" s="132"/>
+      <c r="U17" s="132"/>
     </row>
     <row r="18" spans="3:21" ht="40.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C18" s="138" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="138"/>
-      <c r="E18" s="138"/>
-      <c r="F18" s="138"/>
-      <c r="G18" s="138"/>
-      <c r="H18" s="138"/>
-      <c r="I18" s="138"/>
-      <c r="J18" s="138"/>
-      <c r="K18" s="142" t="s">
+      <c r="C18" s="93" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="93"/>
+      <c r="E18" s="93"/>
+      <c r="F18" s="93"/>
+      <c r="G18" s="93"/>
+      <c r="H18" s="93"/>
+      <c r="I18" s="93"/>
+      <c r="J18" s="93"/>
+      <c r="K18" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="L18" s="143"/>
-      <c r="M18" s="143"/>
-      <c r="N18" s="143"/>
-      <c r="O18" s="143"/>
-      <c r="P18" s="143"/>
-      <c r="Q18" s="143"/>
-      <c r="R18" s="143"/>
-      <c r="S18" s="143"/>
-      <c r="T18" s="143"/>
-      <c r="U18" s="144"/>
+      <c r="L18" s="100"/>
+      <c r="M18" s="100"/>
+      <c r="N18" s="100"/>
+      <c r="O18" s="100"/>
+      <c r="P18" s="100"/>
+      <c r="Q18" s="100"/>
+      <c r="R18" s="100"/>
+      <c r="S18" s="100"/>
+      <c r="T18" s="100"/>
+      <c r="U18" s="101"/>
     </row>
     <row r="19" spans="3:21" ht="27" customHeight="1" x14ac:dyDescent="0.6">
       <c r="C19" s="9"/>
@@ -2179,29 +2243,29 @@
       <c r="U19" s="48"/>
     </row>
     <row r="20" spans="3:21" ht="45" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C20" s="96" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="96"/>
-      <c r="E20" s="96"/>
-      <c r="F20" s="96"/>
-      <c r="G20" s="96"/>
-      <c r="H20" s="96"/>
-      <c r="I20" s="96"/>
-      <c r="J20" s="96"/>
-      <c r="K20" s="131" t="s">
+      <c r="C20" s="133" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="133"/>
+      <c r="E20" s="133"/>
+      <c r="F20" s="133"/>
+      <c r="G20" s="133"/>
+      <c r="H20" s="133"/>
+      <c r="I20" s="133"/>
+      <c r="J20" s="133"/>
+      <c r="K20" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="L20" s="132"/>
-      <c r="M20" s="132"/>
-      <c r="N20" s="132"/>
-      <c r="O20" s="132"/>
-      <c r="P20" s="132"/>
-      <c r="Q20" s="132"/>
-      <c r="R20" s="132"/>
-      <c r="S20" s="132"/>
-      <c r="T20" s="132"/>
-      <c r="U20" s="145"/>
+      <c r="L20" s="103"/>
+      <c r="M20" s="103"/>
+      <c r="N20" s="103"/>
+      <c r="O20" s="103"/>
+      <c r="P20" s="103"/>
+      <c r="Q20" s="103"/>
+      <c r="R20" s="103"/>
+      <c r="S20" s="103"/>
+      <c r="T20" s="103"/>
+      <c r="U20" s="104"/>
     </row>
     <row r="21" spans="3:21" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C21" s="58"/>
@@ -2225,102 +2289,102 @@
       <c r="U21" s="54"/>
     </row>
     <row r="22" spans="3:21" ht="47.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C22" s="88" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="89"/>
-      <c r="E22" s="89"/>
-      <c r="F22" s="89"/>
-      <c r="G22" s="89"/>
-      <c r="H22" s="89"/>
-      <c r="I22" s="89"/>
-      <c r="J22" s="89"/>
-      <c r="K22" s="140" t="s">
+      <c r="C22" s="95" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="96"/>
+      <c r="E22" s="96"/>
+      <c r="F22" s="96"/>
+      <c r="G22" s="96"/>
+      <c r="H22" s="96"/>
+      <c r="I22" s="96"/>
+      <c r="J22" s="96"/>
+      <c r="K22" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="L22" s="140"/>
-      <c r="M22" s="140"/>
-      <c r="N22" s="140"/>
-      <c r="O22" s="140"/>
-      <c r="P22" s="140"/>
-      <c r="Q22" s="140"/>
-      <c r="R22" s="140"/>
-      <c r="S22" s="140"/>
-      <c r="T22" s="140"/>
-      <c r="U22" s="141"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="97"/>
+      <c r="N22" s="97"/>
+      <c r="O22" s="97"/>
+      <c r="P22" s="97"/>
+      <c r="Q22" s="97"/>
+      <c r="R22" s="97"/>
+      <c r="S22" s="97"/>
+      <c r="T22" s="97"/>
+      <c r="U22" s="98"/>
     </row>
     <row r="23" spans="3:21" s="8" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C23" s="123" t="s">
+      <c r="C23" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="123"/>
-      <c r="E23" s="123"/>
-      <c r="F23" s="123"/>
-      <c r="G23" s="107" t="s">
+      <c r="D23" s="107"/>
+      <c r="E23" s="107"/>
+      <c r="F23" s="107"/>
+      <c r="G23" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="H23" s="107"/>
-      <c r="I23" s="107"/>
-      <c r="J23" s="107"/>
-      <c r="K23" s="146" t="s">
+      <c r="H23" s="127"/>
+      <c r="I23" s="127"/>
+      <c r="J23" s="127"/>
+      <c r="K23" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="L23" s="146"/>
-      <c r="M23" s="146"/>
-      <c r="N23" s="146"/>
-      <c r="O23" s="146"/>
-      <c r="P23" s="146"/>
-      <c r="Q23" s="146"/>
-      <c r="R23" s="146"/>
-      <c r="S23" s="146"/>
+      <c r="L23" s="105"/>
+      <c r="M23" s="105"/>
+      <c r="N23" s="105"/>
+      <c r="O23" s="105"/>
+      <c r="P23" s="105"/>
+      <c r="Q23" s="105"/>
+      <c r="R23" s="105"/>
+      <c r="S23" s="105"/>
       <c r="T23" s="12"/>
       <c r="U23" s="7"/>
     </row>
     <row r="24" spans="3:21" ht="55.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C24" s="103" t="s">
+      <c r="C24" s="123" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="103"/>
-      <c r="E24" s="103"/>
-      <c r="F24" s="103"/>
-      <c r="G24" s="103"/>
-      <c r="H24" s="103"/>
-      <c r="I24" s="103"/>
-      <c r="J24" s="103"/>
-      <c r="K24" s="103"/>
-      <c r="L24" s="103"/>
-      <c r="M24" s="103"/>
-      <c r="N24" s="103"/>
-      <c r="O24" s="103"/>
-      <c r="P24" s="103"/>
-      <c r="Q24" s="103"/>
-      <c r="R24" s="103"/>
-      <c r="S24" s="103"/>
-      <c r="T24" s="103"/>
-      <c r="U24" s="103"/>
+      <c r="D24" s="123"/>
+      <c r="E24" s="123"/>
+      <c r="F24" s="123"/>
+      <c r="G24" s="123"/>
+      <c r="H24" s="123"/>
+      <c r="I24" s="123"/>
+      <c r="J24" s="123"/>
+      <c r="K24" s="123"/>
+      <c r="L24" s="123"/>
+      <c r="M24" s="123"/>
+      <c r="N24" s="123"/>
+      <c r="O24" s="123"/>
+      <c r="P24" s="123"/>
+      <c r="Q24" s="123"/>
+      <c r="R24" s="123"/>
+      <c r="S24" s="123"/>
+      <c r="T24" s="123"/>
+      <c r="U24" s="123"/>
     </row>
     <row r="25" spans="3:21" ht="30" x14ac:dyDescent="0.55000000000000004">
-      <c r="C25" s="122" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="122"/>
-      <c r="E25" s="122"/>
-      <c r="F25" s="122"/>
-      <c r="G25" s="122"/>
-      <c r="H25" s="122"/>
-      <c r="I25" s="122"/>
-      <c r="J25" s="122"/>
-      <c r="K25" s="122"/>
-      <c r="L25" s="122"/>
-      <c r="M25" s="122"/>
-      <c r="N25" s="122"/>
-      <c r="O25" s="122"/>
-      <c r="P25" s="122"/>
-      <c r="Q25" s="122"/>
-      <c r="R25" s="122"/>
-      <c r="S25" s="122"/>
-      <c r="T25" s="122"/>
-      <c r="U25" s="122"/>
+      <c r="C25" s="106" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="106"/>
+      <c r="E25" s="106"/>
+      <c r="F25" s="106"/>
+      <c r="G25" s="106"/>
+      <c r="H25" s="106"/>
+      <c r="I25" s="106"/>
+      <c r="J25" s="106"/>
+      <c r="K25" s="106"/>
+      <c r="L25" s="106"/>
+      <c r="M25" s="106"/>
+      <c r="N25" s="106"/>
+      <c r="O25" s="106"/>
+      <c r="P25" s="106"/>
+      <c r="Q25" s="106"/>
+      <c r="R25" s="106"/>
+      <c r="S25" s="106"/>
+      <c r="T25" s="106"/>
+      <c r="U25" s="106"/>
     </row>
     <row r="26" spans="3:21" ht="4.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C26" s="13"/>
@@ -2342,27 +2406,27 @@
       <c r="U26" s="13"/>
     </row>
     <row r="27" spans="3:21" ht="30" x14ac:dyDescent="0.55000000000000004">
-      <c r="C27" s="75" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="75"/>
-      <c r="H27" s="75"/>
-      <c r="I27" s="75"/>
-      <c r="J27" s="75"/>
-      <c r="K27" s="75"/>
-      <c r="L27" s="75"/>
-      <c r="M27" s="75"/>
-      <c r="N27" s="75"/>
-      <c r="O27" s="75"/>
-      <c r="P27" s="75"/>
-      <c r="Q27" s="75"/>
-      <c r="R27" s="75"/>
-      <c r="S27" s="75"/>
-      <c r="T27" s="75"/>
-      <c r="U27" s="75"/>
+      <c r="C27" s="151" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="151"/>
+      <c r="E27" s="151"/>
+      <c r="F27" s="151"/>
+      <c r="G27" s="151"/>
+      <c r="H27" s="151"/>
+      <c r="I27" s="151"/>
+      <c r="J27" s="151"/>
+      <c r="K27" s="151"/>
+      <c r="L27" s="151"/>
+      <c r="M27" s="151"/>
+      <c r="N27" s="151"/>
+      <c r="O27" s="151"/>
+      <c r="P27" s="151"/>
+      <c r="Q27" s="151"/>
+      <c r="R27" s="151"/>
+      <c r="S27" s="151"/>
+      <c r="T27" s="151"/>
+      <c r="U27" s="151"/>
     </row>
     <row r="28" spans="3:21" ht="15" customHeight="1" x14ac:dyDescent="0.6">
       <c r="C28" s="14"/>
@@ -2428,89 +2492,89 @@
       <c r="U30" s="2"/>
     </row>
     <row r="31" spans="3:21" ht="30" x14ac:dyDescent="0.6">
-      <c r="C31" s="87" t="s">
+      <c r="C31" s="158" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="87"/>
-      <c r="E31" s="87"/>
-      <c r="F31" s="87"/>
-      <c r="G31" s="87"/>
-      <c r="H31" s="87"/>
-      <c r="I31" s="87"/>
-      <c r="J31" s="87"/>
-      <c r="K31" s="87"/>
-      <c r="L31" s="87"/>
-      <c r="M31" s="87"/>
-      <c r="N31" s="87"/>
-      <c r="O31" s="87"/>
-      <c r="P31" s="87"/>
-      <c r="Q31" s="87"/>
-      <c r="R31" s="87"/>
-      <c r="S31" s="87"/>
-      <c r="T31" s="87"/>
-      <c r="U31" s="87"/>
+      <c r="D31" s="158"/>
+      <c r="E31" s="158"/>
+      <c r="F31" s="158"/>
+      <c r="G31" s="158"/>
+      <c r="H31" s="158"/>
+      <c r="I31" s="158"/>
+      <c r="J31" s="158"/>
+      <c r="K31" s="158"/>
+      <c r="L31" s="158"/>
+      <c r="M31" s="158"/>
+      <c r="N31" s="158"/>
+      <c r="O31" s="158"/>
+      <c r="P31" s="158"/>
+      <c r="Q31" s="158"/>
+      <c r="R31" s="158"/>
+      <c r="S31" s="158"/>
+      <c r="T31" s="158"/>
+      <c r="U31" s="158"/>
     </row>
     <row r="32" spans="3:21" ht="30" x14ac:dyDescent="0.6">
-      <c r="C32" s="101"/>
-      <c r="D32" s="101"/>
-      <c r="E32" s="102"/>
-      <c r="F32" s="102"/>
-      <c r="G32" s="102"/>
-      <c r="H32" s="102"/>
-      <c r="I32" s="102"/>
-      <c r="J32" s="101"/>
-      <c r="K32" s="101"/>
-      <c r="L32" s="101"/>
-      <c r="M32" s="101"/>
-      <c r="N32" s="101"/>
-      <c r="O32" s="101"/>
-      <c r="P32" s="101"/>
-      <c r="Q32" s="101"/>
-      <c r="R32" s="101"/>
-      <c r="S32" s="101"/>
-      <c r="T32" s="101"/>
+      <c r="C32" s="122"/>
+      <c r="D32" s="122"/>
+      <c r="E32" s="115"/>
+      <c r="F32" s="115"/>
+      <c r="G32" s="115"/>
+      <c r="H32" s="115"/>
+      <c r="I32" s="115"/>
+      <c r="J32" s="122"/>
+      <c r="K32" s="122"/>
+      <c r="L32" s="122"/>
+      <c r="M32" s="122"/>
+      <c r="N32" s="122"/>
+      <c r="O32" s="122"/>
+      <c r="P32" s="122"/>
+      <c r="Q32" s="122"/>
+      <c r="R32" s="122"/>
+      <c r="S32" s="122"/>
+      <c r="T32" s="122"/>
       <c r="U32" s="2"/>
     </row>
     <row r="33" spans="3:22" ht="71.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C33" s="86" t="s">
+      <c r="C33" s="113" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="86"/>
-      <c r="E33" s="86"/>
-      <c r="F33" s="86"/>
-      <c r="G33" s="86"/>
-      <c r="H33" s="86"/>
-      <c r="I33" s="86"/>
-      <c r="J33" s="86"/>
-      <c r="K33" s="86"/>
-      <c r="L33" s="86"/>
-      <c r="M33" s="86"/>
-      <c r="N33" s="86"/>
-      <c r="O33" s="86"/>
-      <c r="P33" s="86"/>
-      <c r="Q33" s="86"/>
-      <c r="R33" s="86"/>
-      <c r="S33" s="86"/>
-      <c r="T33" s="86"/>
-      <c r="U33" s="86"/>
+      <c r="D33" s="113"/>
+      <c r="E33" s="113"/>
+      <c r="F33" s="113"/>
+      <c r="G33" s="113"/>
+      <c r="H33" s="113"/>
+      <c r="I33" s="113"/>
+      <c r="J33" s="113"/>
+      <c r="K33" s="113"/>
+      <c r="L33" s="113"/>
+      <c r="M33" s="113"/>
+      <c r="N33" s="113"/>
+      <c r="O33" s="113"/>
+      <c r="P33" s="113"/>
+      <c r="Q33" s="113"/>
+      <c r="R33" s="113"/>
+      <c r="S33" s="113"/>
+      <c r="T33" s="113"/>
+      <c r="U33" s="113"/>
     </row>
     <row r="34" spans="3:22" ht="70.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="C34" s="86" t="s">
+      <c r="C34" s="113" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="86"/>
-      <c r="E34" s="86"/>
-      <c r="F34" s="86"/>
-      <c r="G34" s="86"/>
-      <c r="H34" s="86"/>
-      <c r="I34" s="86"/>
-      <c r="J34" s="86"/>
-      <c r="K34" s="86"/>
-      <c r="L34" s="86"/>
-      <c r="M34" s="86"/>
-      <c r="N34" s="86"/>
-      <c r="O34" s="86"/>
-      <c r="P34" s="86"/>
+      <c r="D34" s="113"/>
+      <c r="E34" s="113"/>
+      <c r="F34" s="113"/>
+      <c r="G34" s="113"/>
+      <c r="H34" s="113"/>
+      <c r="I34" s="113"/>
+      <c r="J34" s="113"/>
+      <c r="K34" s="113"/>
+      <c r="L34" s="113"/>
+      <c r="M34" s="113"/>
+      <c r="N34" s="113"/>
+      <c r="O34" s="113"/>
+      <c r="P34" s="113"/>
       <c r="Q34" s="17"/>
       <c r="R34" s="17"/>
       <c r="S34" s="18"/>
@@ -2568,19 +2632,19 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
-      <c r="K37" s="80" t="s">
+      <c r="K37" s="114" t="s">
         <v>29</v>
       </c>
-      <c r="L37" s="80"/>
-      <c r="M37" s="80"/>
-      <c r="N37" s="80"/>
-      <c r="O37" s="80"/>
-      <c r="P37" s="80"/>
-      <c r="Q37" s="80"/>
-      <c r="R37" s="80"/>
-      <c r="S37" s="80"/>
-      <c r="T37" s="80"/>
-      <c r="U37" s="80"/>
+      <c r="L37" s="114"/>
+      <c r="M37" s="114"/>
+      <c r="N37" s="114"/>
+      <c r="O37" s="114"/>
+      <c r="P37" s="114"/>
+      <c r="Q37" s="114"/>
+      <c r="R37" s="114"/>
+      <c r="S37" s="114"/>
+      <c r="T37" s="114"/>
+      <c r="U37" s="114"/>
     </row>
     <row r="38" spans="3:22" ht="3" customHeight="1" x14ac:dyDescent="0.6">
       <c r="C38" s="2"/>
@@ -2615,7 +2679,7 @@
       <c r="K39" s="21"/>
       <c r="L39" s="21"/>
       <c r="M39" s="41" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N39" s="21"/>
       <c r="O39" s="21"/>
@@ -2669,162 +2733,162 @@
       <c r="U41" s="2"/>
     </row>
     <row r="42" spans="3:22" ht="30.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="C42" s="78" t="s">
+      <c r="C42" s="154" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" s="154"/>
+      <c r="E42" s="154"/>
+      <c r="F42" s="154"/>
+      <c r="G42" s="154"/>
+      <c r="H42" s="154"/>
+      <c r="I42" s="154"/>
+      <c r="J42" s="154"/>
+      <c r="K42" s="154"/>
+      <c r="L42" s="154"/>
+      <c r="M42" s="154"/>
+      <c r="N42" s="154"/>
+      <c r="O42" s="154"/>
+      <c r="P42" s="154"/>
+      <c r="Q42" s="154"/>
+      <c r="R42" s="154"/>
+      <c r="S42" s="154"/>
+      <c r="T42" s="154"/>
+      <c r="U42" s="154"/>
+    </row>
+    <row r="43" spans="3:22" ht="26" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C43" s="112" t="s">
+        <v>39</v>
+      </c>
+      <c r="D43" s="112"/>
+      <c r="E43" s="112"/>
+      <c r="F43" s="112"/>
+      <c r="G43" s="112"/>
+      <c r="H43" s="112"/>
+      <c r="I43" s="112"/>
+      <c r="J43" s="112"/>
+      <c r="K43" s="112"/>
+      <c r="L43" s="112"/>
+      <c r="M43" s="112"/>
+      <c r="N43" s="112"/>
+      <c r="O43" s="112"/>
+      <c r="P43" s="112"/>
+      <c r="Q43" s="112"/>
+      <c r="R43" s="112"/>
+      <c r="S43" s="112"/>
+      <c r="T43" s="112"/>
+      <c r="U43" s="112"/>
+    </row>
+    <row r="44" spans="3:22" ht="30.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C44" s="94" t="s">
+        <v>38</v>
+      </c>
+      <c r="D44" s="94"/>
+      <c r="E44" s="94"/>
+      <c r="F44" s="94"/>
+      <c r="G44" s="94"/>
+      <c r="H44" s="94"/>
+      <c r="I44" s="94"/>
+      <c r="J44" s="94"/>
+      <c r="K44" s="94"/>
+      <c r="L44" s="94"/>
+      <c r="M44" s="94"/>
+      <c r="N44" s="94"/>
+      <c r="O44" s="94"/>
+      <c r="P44" s="94"/>
+      <c r="Q44" s="94"/>
+      <c r="R44" s="94"/>
+      <c r="S44" s="94"/>
+      <c r="T44" s="94"/>
+      <c r="U44" s="94"/>
+    </row>
+    <row r="45" spans="3:22" ht="30.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C45" s="94"/>
+      <c r="D45" s="94"/>
+      <c r="E45" s="94"/>
+      <c r="F45" s="94"/>
+      <c r="G45" s="94"/>
+      <c r="H45" s="94"/>
+      <c r="I45" s="94"/>
+      <c r="J45" s="94"/>
+      <c r="K45" s="94"/>
+      <c r="L45" s="94"/>
+      <c r="M45" s="94"/>
+      <c r="N45" s="94"/>
+      <c r="O45" s="94"/>
+      <c r="P45" s="94"/>
+      <c r="Q45" s="94"/>
+      <c r="R45" s="94"/>
+      <c r="S45" s="94"/>
+      <c r="T45" s="94"/>
+      <c r="U45" s="94"/>
+    </row>
+    <row r="46" spans="3:22" ht="31" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C46" s="94"/>
+      <c r="D46" s="94"/>
+      <c r="E46" s="94"/>
+      <c r="F46" s="94"/>
+      <c r="G46" s="94"/>
+      <c r="H46" s="94"/>
+      <c r="I46" s="94"/>
+      <c r="J46" s="94"/>
+      <c r="K46" s="94"/>
+      <c r="L46" s="94"/>
+      <c r="M46" s="94"/>
+      <c r="N46" s="94"/>
+      <c r="O46" s="94"/>
+      <c r="P46" s="94"/>
+      <c r="Q46" s="94"/>
+      <c r="R46" s="94"/>
+      <c r="S46" s="94"/>
+      <c r="T46" s="94"/>
+      <c r="U46" s="94"/>
+    </row>
+    <row r="47" spans="3:22" ht="31" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C47" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="D42" s="78"/>
-      <c r="E42" s="78"/>
-      <c r="F42" s="78"/>
-      <c r="G42" s="78"/>
-      <c r="H42" s="78"/>
-      <c r="I42" s="78"/>
-      <c r="J42" s="78"/>
-      <c r="K42" s="78"/>
-      <c r="L42" s="78"/>
-      <c r="M42" s="78"/>
-      <c r="N42" s="78"/>
-      <c r="O42" s="78"/>
-      <c r="P42" s="78"/>
-      <c r="Q42" s="78"/>
-      <c r="R42" s="78"/>
-      <c r="S42" s="78"/>
-      <c r="T42" s="78"/>
-      <c r="U42" s="78"/>
-    </row>
-    <row r="43" spans="3:22" ht="26" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C43" s="127" t="s">
-        <v>42</v>
-      </c>
-      <c r="D43" s="127"/>
-      <c r="E43" s="127"/>
-      <c r="F43" s="127"/>
-      <c r="G43" s="127"/>
-      <c r="H43" s="127"/>
-      <c r="I43" s="127"/>
-      <c r="J43" s="127"/>
-      <c r="K43" s="127"/>
-      <c r="L43" s="127"/>
-      <c r="M43" s="127"/>
-      <c r="N43" s="127"/>
-      <c r="O43" s="127"/>
-      <c r="P43" s="127"/>
-      <c r="Q43" s="127"/>
-      <c r="R43" s="127"/>
-      <c r="S43" s="127"/>
-      <c r="T43" s="127"/>
-      <c r="U43" s="127"/>
-    </row>
-    <row r="44" spans="3:22" ht="30.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C44" s="139" t="s">
-        <v>41</v>
-      </c>
-      <c r="D44" s="139"/>
-      <c r="E44" s="139"/>
-      <c r="F44" s="139"/>
-      <c r="G44" s="139"/>
-      <c r="H44" s="139"/>
-      <c r="I44" s="139"/>
-      <c r="J44" s="139"/>
-      <c r="K44" s="139"/>
-      <c r="L44" s="139"/>
-      <c r="M44" s="139"/>
-      <c r="N44" s="139"/>
-      <c r="O44" s="139"/>
-      <c r="P44" s="139"/>
-      <c r="Q44" s="139"/>
-      <c r="R44" s="139"/>
-      <c r="S44" s="139"/>
-      <c r="T44" s="139"/>
-      <c r="U44" s="139"/>
-    </row>
-    <row r="45" spans="3:22" ht="30.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C45" s="139"/>
-      <c r="D45" s="139"/>
-      <c r="E45" s="139"/>
-      <c r="F45" s="139"/>
-      <c r="G45" s="139"/>
-      <c r="H45" s="139"/>
-      <c r="I45" s="139"/>
-      <c r="J45" s="139"/>
-      <c r="K45" s="139"/>
-      <c r="L45" s="139"/>
-      <c r="M45" s="139"/>
-      <c r="N45" s="139"/>
-      <c r="O45" s="139"/>
-      <c r="P45" s="139"/>
-      <c r="Q45" s="139"/>
-      <c r="R45" s="139"/>
-      <c r="S45" s="139"/>
-      <c r="T45" s="139"/>
-      <c r="U45" s="139"/>
-    </row>
-    <row r="46" spans="3:22" ht="31" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C46" s="139"/>
-      <c r="D46" s="139"/>
-      <c r="E46" s="139"/>
-      <c r="F46" s="139"/>
-      <c r="G46" s="139"/>
-      <c r="H46" s="139"/>
-      <c r="I46" s="139"/>
-      <c r="J46" s="139"/>
-      <c r="K46" s="139"/>
-      <c r="L46" s="139"/>
-      <c r="M46" s="139"/>
-      <c r="N46" s="139"/>
-      <c r="O46" s="139"/>
-      <c r="P46" s="139"/>
-      <c r="Q46" s="139"/>
-      <c r="R46" s="139"/>
-      <c r="S46" s="139"/>
-      <c r="T46" s="139"/>
-      <c r="U46" s="139"/>
-    </row>
-    <row r="47" spans="3:22" ht="31" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C47" s="136" t="s">
-        <v>43</v>
-      </c>
-      <c r="D47" s="136"/>
-      <c r="E47" s="136"/>
-      <c r="F47" s="136"/>
-      <c r="G47" s="136"/>
-      <c r="H47" s="136"/>
-      <c r="I47" s="136"/>
-      <c r="J47" s="136"/>
-      <c r="K47" s="136"/>
-      <c r="L47" s="136"/>
-      <c r="M47" s="136"/>
-      <c r="N47" s="136"/>
-      <c r="O47" s="136"/>
-      <c r="P47" s="136"/>
-      <c r="Q47" s="136"/>
-      <c r="R47" s="136"/>
-      <c r="S47" s="136"/>
-      <c r="T47" s="136"/>
-      <c r="U47" s="136"/>
+      <c r="D47" s="89"/>
+      <c r="E47" s="89"/>
+      <c r="F47" s="89"/>
+      <c r="G47" s="89"/>
+      <c r="H47" s="89"/>
+      <c r="I47" s="89"/>
+      <c r="J47" s="89"/>
+      <c r="K47" s="89"/>
+      <c r="L47" s="89"/>
+      <c r="M47" s="89"/>
+      <c r="N47" s="89"/>
+      <c r="O47" s="89"/>
+      <c r="P47" s="89"/>
+      <c r="Q47" s="89"/>
+      <c r="R47" s="89"/>
+      <c r="S47" s="89"/>
+      <c r="T47" s="89"/>
+      <c r="U47" s="89"/>
     </row>
     <row r="48" spans="3:22" ht="30.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="C48" s="126" t="s">
-        <v>39</v>
-      </c>
-      <c r="D48" s="126"/>
-      <c r="E48" s="126"/>
-      <c r="F48" s="126"/>
-      <c r="G48" s="126"/>
-      <c r="H48" s="126"/>
-      <c r="I48" s="126"/>
-      <c r="J48" s="126"/>
-      <c r="K48" s="126"/>
-      <c r="L48" s="126"/>
-      <c r="M48" s="126"/>
-      <c r="N48" s="126"/>
-      <c r="O48" s="126"/>
-      <c r="P48" s="126"/>
-      <c r="Q48" s="126"/>
-      <c r="R48" s="126"/>
-      <c r="S48" s="126"/>
-      <c r="T48" s="126"/>
-      <c r="U48" s="126"/>
-      <c r="V48" s="126"/>
+      <c r="C48" s="111" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48" s="111"/>
+      <c r="E48" s="111"/>
+      <c r="F48" s="111"/>
+      <c r="G48" s="111"/>
+      <c r="H48" s="111"/>
+      <c r="I48" s="111"/>
+      <c r="J48" s="111"/>
+      <c r="K48" s="111"/>
+      <c r="L48" s="111"/>
+      <c r="M48" s="111"/>
+      <c r="N48" s="111"/>
+      <c r="O48" s="111"/>
+      <c r="P48" s="111"/>
+      <c r="Q48" s="111"/>
+      <c r="R48" s="111"/>
+      <c r="S48" s="111"/>
+      <c r="T48" s="111"/>
+      <c r="U48" s="111"/>
+      <c r="V48" s="111"/>
     </row>
     <row r="49" spans="3:32" ht="30.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="C49" s="28"/>
@@ -2895,27 +2959,27 @@
       <c r="AD51" s="30"/>
     </row>
     <row r="52" spans="3:32" x14ac:dyDescent="0.55000000000000004">
-      <c r="C52" s="125" t="s">
-        <v>33</v>
-      </c>
-      <c r="D52" s="125"/>
-      <c r="E52" s="125"/>
-      <c r="F52" s="125"/>
-      <c r="G52" s="125"/>
-      <c r="H52" s="125"/>
-      <c r="I52" s="125"/>
-      <c r="J52" s="125"/>
-      <c r="K52" s="125"/>
-      <c r="L52" s="125"/>
-      <c r="M52" s="125"/>
-      <c r="N52" s="125"/>
-      <c r="O52" s="125"/>
-      <c r="P52" s="125"/>
-      <c r="Q52" s="125"/>
-      <c r="R52" s="125"/>
-      <c r="S52" s="125"/>
-      <c r="T52" s="125"/>
-      <c r="U52" s="125"/>
+      <c r="C52" s="110" t="s">
+        <v>58</v>
+      </c>
+      <c r="D52" s="110"/>
+      <c r="E52" s="110"/>
+      <c r="F52" s="110"/>
+      <c r="G52" s="110"/>
+      <c r="H52" s="110"/>
+      <c r="I52" s="110"/>
+      <c r="J52" s="110"/>
+      <c r="K52" s="110"/>
+      <c r="L52" s="110"/>
+      <c r="M52" s="110"/>
+      <c r="N52" s="110"/>
+      <c r="O52" s="110"/>
+      <c r="P52" s="110"/>
+      <c r="Q52" s="110"/>
+      <c r="R52" s="110"/>
+      <c r="S52" s="110"/>
+      <c r="T52" s="110"/>
+      <c r="U52" s="110"/>
       <c r="Z52" s="30"/>
       <c r="AA52" s="30"/>
       <c r="AB52" s="30"/>
@@ -2923,49 +2987,49 @@
       <c r="AD52" s="30"/>
     </row>
     <row r="53" spans="3:32" ht="52" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C53" s="124" t="s">
+      <c r="C53" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="D53" s="124"/>
-      <c r="E53" s="124"/>
-      <c r="F53" s="124"/>
-      <c r="G53" s="124"/>
-      <c r="H53" s="124"/>
-      <c r="I53" s="124"/>
-      <c r="J53" s="124"/>
-      <c r="K53" s="124"/>
-      <c r="L53" s="124"/>
-      <c r="M53" s="124"/>
-      <c r="N53" s="124"/>
-      <c r="O53" s="124"/>
-      <c r="P53" s="124"/>
-      <c r="Q53" s="124"/>
-      <c r="R53" s="124"/>
-      <c r="S53" s="124"/>
-      <c r="T53" s="124"/>
-      <c r="U53" s="124"/>
+      <c r="D53" s="109"/>
+      <c r="E53" s="109"/>
+      <c r="F53" s="109"/>
+      <c r="G53" s="109"/>
+      <c r="H53" s="109"/>
+      <c r="I53" s="109"/>
+      <c r="J53" s="109"/>
+      <c r="K53" s="109"/>
+      <c r="L53" s="109"/>
+      <c r="M53" s="109"/>
+      <c r="N53" s="109"/>
+      <c r="O53" s="109"/>
+      <c r="P53" s="109"/>
+      <c r="Q53" s="109"/>
+      <c r="R53" s="109"/>
+      <c r="S53" s="109"/>
+      <c r="T53" s="109"/>
+      <c r="U53" s="109"/>
       <c r="Z53" s="30"/>
-      <c r="AA53" s="129"/>
-      <c r="AB53" s="129"/>
-      <c r="AC53" s="129"/>
+      <c r="AA53" s="85"/>
+      <c r="AB53" s="85"/>
+      <c r="AC53" s="85"/>
       <c r="AD53" s="30"/>
     </row>
     <row r="54" spans="3:32" ht="1.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="C54" s="79"/>
-      <c r="D54" s="79"/>
-      <c r="E54" s="79"/>
-      <c r="F54" s="79"/>
-      <c r="G54" s="79"/>
-      <c r="H54" s="79"/>
-      <c r="I54" s="79"/>
-      <c r="J54" s="79"/>
-      <c r="K54" s="79"/>
-      <c r="L54" s="79"/>
-      <c r="M54" s="79"/>
-      <c r="N54" s="79"/>
-      <c r="O54" s="79"/>
-      <c r="P54" s="79"/>
-      <c r="Q54" s="79"/>
+      <c r="C54" s="108"/>
+      <c r="D54" s="108"/>
+      <c r="E54" s="108"/>
+      <c r="F54" s="108"/>
+      <c r="G54" s="108"/>
+      <c r="H54" s="108"/>
+      <c r="I54" s="108"/>
+      <c r="J54" s="108"/>
+      <c r="K54" s="108"/>
+      <c r="L54" s="108"/>
+      <c r="M54" s="108"/>
+      <c r="N54" s="108"/>
+      <c r="O54" s="108"/>
+      <c r="P54" s="108"/>
+      <c r="Q54" s="108"/>
       <c r="R54" s="2"/>
       <c r="S54" s="2"/>
       <c r="T54" s="2"/>
@@ -2977,20 +3041,20 @@
       <c r="AD54" s="30"/>
     </row>
     <row r="55" spans="3:32" ht="3.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="C55" s="79"/>
-      <c r="D55" s="79"/>
-      <c r="E55" s="79"/>
-      <c r="F55" s="79"/>
-      <c r="G55" s="79"/>
-      <c r="H55" s="79"/>
-      <c r="I55" s="79"/>
-      <c r="J55" s="79"/>
-      <c r="K55" s="79"/>
-      <c r="L55" s="79"/>
-      <c r="M55" s="79"/>
-      <c r="N55" s="79"/>
-      <c r="O55" s="79"/>
-      <c r="P55" s="79"/>
+      <c r="C55" s="108"/>
+      <c r="D55" s="108"/>
+      <c r="E55" s="108"/>
+      <c r="F55" s="108"/>
+      <c r="G55" s="108"/>
+      <c r="H55" s="108"/>
+      <c r="I55" s="108"/>
+      <c r="J55" s="108"/>
+      <c r="K55" s="108"/>
+      <c r="L55" s="108"/>
+      <c r="M55" s="108"/>
+      <c r="N55" s="108"/>
+      <c r="O55" s="108"/>
+      <c r="P55" s="108"/>
       <c r="Q55" s="2"/>
       <c r="R55" s="2"/>
       <c r="S55" s="2"/>
@@ -3004,7 +3068,7 @@
     </row>
     <row r="56" spans="3:32" ht="30" x14ac:dyDescent="0.55000000000000004">
       <c r="C56" s="4" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
@@ -3069,32 +3133,32 @@
       </c>
       <c r="H58" s="70"/>
       <c r="I58" s="69" t="s">
-        <v>46</v>
-      </c>
-      <c r="J58" s="97" t="s">
+        <v>43</v>
+      </c>
+      <c r="J58" s="139" t="s">
         <v>3</v>
       </c>
-      <c r="K58" s="97"/>
-      <c r="L58" s="99" t="s">
-        <v>58</v>
-      </c>
-      <c r="M58" s="99"/>
-      <c r="N58" s="99"/>
-      <c r="O58" s="99"/>
-      <c r="P58" s="99" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q58" s="99"/>
-      <c r="R58" s="99"/>
-      <c r="S58" s="99"/>
-      <c r="T58" s="99"/>
-      <c r="U58" s="99"/>
+      <c r="K58" s="139"/>
+      <c r="L58" s="141" t="s">
+        <v>55</v>
+      </c>
+      <c r="M58" s="142"/>
+      <c r="N58" s="142"/>
+      <c r="O58" s="143"/>
+      <c r="P58" s="148" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q58" s="148"/>
+      <c r="R58" s="148"/>
+      <c r="S58" s="148"/>
+      <c r="T58" s="148"/>
+      <c r="U58" s="148"/>
       <c r="V58" s="52"/>
       <c r="Y58" s="42"/>
       <c r="Z58" s="42"/>
-      <c r="AA58" s="92"/>
-      <c r="AB58" s="92"/>
-      <c r="AC58" s="92"/>
+      <c r="AA58" s="136"/>
+      <c r="AB58" s="136"/>
+      <c r="AC58" s="136"/>
       <c r="AD58" s="42"/>
       <c r="AE58" s="42"/>
       <c r="AF58" s="42"/>
@@ -3103,40 +3167,40 @@
       <c r="C59" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="D59" s="81" t="s">
+      <c r="D59" s="155" t="s">
         <v>13</v>
       </c>
-      <c r="E59" s="81"/>
-      <c r="F59" s="81"/>
-      <c r="G59" s="73" t="s">
+      <c r="E59" s="155"/>
+      <c r="F59" s="155"/>
+      <c r="G59" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="H59" s="71"/>
-      <c r="I59" s="72" t="s">
+      <c r="H59" s="72"/>
+      <c r="I59" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="J59" s="98" t="s">
+      <c r="J59" s="140" t="s">
         <v>14</v>
       </c>
-      <c r="K59" s="98"/>
-      <c r="L59" s="98" t="s">
+      <c r="K59" s="140"/>
+      <c r="L59" s="140" t="s">
         <v>20</v>
       </c>
-      <c r="M59" s="98"/>
-      <c r="N59" s="98"/>
-      <c r="O59" s="98"/>
-      <c r="P59" s="128" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q59" s="128"/>
-      <c r="R59" s="128"/>
-      <c r="S59" s="128"/>
-      <c r="T59" s="128"/>
-      <c r="U59" s="128"/>
+      <c r="M59" s="140"/>
+      <c r="N59" s="140"/>
+      <c r="O59" s="140"/>
+      <c r="P59" s="140" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q59" s="140"/>
+      <c r="R59" s="140"/>
+      <c r="S59" s="140"/>
+      <c r="T59" s="140"/>
+      <c r="U59" s="140"/>
       <c r="V59" s="60"/>
-      <c r="Y59" s="121"/>
-      <c r="Z59" s="121"/>
-      <c r="AA59" s="121"/>
+      <c r="Y59" s="147"/>
+      <c r="Z59" s="147"/>
+      <c r="AA59" s="147"/>
       <c r="AB59" s="62"/>
       <c r="AC59" s="62"/>
       <c r="AD59" s="62"/>
@@ -3146,8 +3210,8 @@
     <row r="60" spans="3:32" ht="10.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
-      <c r="E60" s="94"/>
-      <c r="F60" s="94"/>
+      <c r="E60" s="138"/>
+      <c r="F60" s="138"/>
       <c r="N60" s="30"/>
       <c r="O60" s="30"/>
       <c r="P60" s="30"/>
@@ -3195,31 +3259,31 @@
       <c r="AF61" s="30"/>
     </row>
     <row r="62" spans="3:32" ht="37.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C62" s="147" t="s">
-        <v>50</v>
-      </c>
-      <c r="D62" s="148"/>
-      <c r="E62" s="148"/>
-      <c r="F62" s="148"/>
-      <c r="G62" s="148"/>
-      <c r="H62" s="148"/>
-      <c r="I62" s="149"/>
-      <c r="J62" s="131" t="s">
+      <c r="C62" s="144" t="s">
+        <v>47</v>
+      </c>
+      <c r="D62" s="145"/>
+      <c r="E62" s="145"/>
+      <c r="F62" s="145"/>
+      <c r="G62" s="145"/>
+      <c r="H62" s="145"/>
+      <c r="I62" s="146"/>
+      <c r="J62" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="K62" s="132"/>
-      <c r="L62" s="132"/>
-      <c r="M62" s="130" t="s">
+      <c r="K62" s="103"/>
+      <c r="L62" s="149" t="s">
         <v>23</v>
       </c>
-      <c r="N62" s="130"/>
-      <c r="O62" s="130"/>
-      <c r="P62" s="130"/>
-      <c r="Q62" s="130"/>
-      <c r="R62" s="130"/>
-      <c r="S62" s="130"/>
-      <c r="T62" s="130"/>
-      <c r="U62" s="130"/>
+      <c r="M62" s="149"/>
+      <c r="N62" s="149"/>
+      <c r="O62" s="149"/>
+      <c r="P62" s="149"/>
+      <c r="Q62" s="149"/>
+      <c r="R62" s="149"/>
+      <c r="S62" s="149"/>
+      <c r="T62" s="149"/>
+      <c r="U62" s="149"/>
       <c r="V62" s="53"/>
       <c r="Y62" s="30"/>
       <c r="Z62" s="30"/>
@@ -3289,29 +3353,29 @@
       <c r="AF64" s="30"/>
     </row>
     <row r="65" spans="2:32" ht="34.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C65" s="96" t="s">
-        <v>45</v>
-      </c>
-      <c r="D65" s="96"/>
-      <c r="E65" s="96"/>
-      <c r="F65" s="96"/>
-      <c r="G65" s="96"/>
-      <c r="H65" s="96"/>
-      <c r="I65" s="96"/>
-      <c r="J65" s="96"/>
-      <c r="K65" s="95" t="s">
+      <c r="C65" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="D65" s="77"/>
+      <c r="E65" s="77"/>
+      <c r="F65" s="77"/>
+      <c r="G65" s="77"/>
+      <c r="H65" s="77"/>
+      <c r="I65" s="78"/>
+      <c r="J65" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="L65" s="95"/>
-      <c r="M65" s="95"/>
-      <c r="N65" s="95"/>
-      <c r="O65" s="95"/>
-      <c r="P65" s="95"/>
-      <c r="Q65" s="95"/>
-      <c r="R65" s="95"/>
-      <c r="S65" s="95"/>
-      <c r="T65" s="95"/>
-      <c r="U65" s="95"/>
+      <c r="K65" s="74"/>
+      <c r="L65" s="74"/>
+      <c r="M65" s="74"/>
+      <c r="N65" s="74"/>
+      <c r="O65" s="74"/>
+      <c r="P65" s="74"/>
+      <c r="Q65" s="74"/>
+      <c r="R65" s="74"/>
+      <c r="S65" s="74"/>
+      <c r="T65" s="74"/>
+      <c r="U65" s="75"/>
       <c r="Y65" s="30"/>
       <c r="Z65" s="30"/>
       <c r="AA65" s="30"/>
@@ -3350,38 +3414,38 @@
       <c r="AE66" s="30"/>
       <c r="AF66" s="30"/>
     </row>
-    <row r="67" spans="2:32" s="40" customFormat="1" ht="43" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C67" s="88" t="s">
+    <row r="67" spans="2:32" s="40" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C67" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="D67" s="89"/>
-      <c r="E67" s="89"/>
-      <c r="F67" s="89"/>
-      <c r="G67" s="89"/>
-      <c r="H67" s="89"/>
-      <c r="I67" s="89"/>
-      <c r="J67" s="89"/>
-      <c r="K67" s="84" t="s">
+      <c r="D67" s="83"/>
+      <c r="E67" s="83"/>
+      <c r="F67" s="83"/>
+      <c r="G67" s="83"/>
+      <c r="H67" s="83"/>
+      <c r="I67" s="84"/>
+      <c r="J67" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="L67" s="84"/>
-      <c r="M67" s="84"/>
-      <c r="N67" s="84"/>
-      <c r="O67" s="84"/>
-      <c r="P67" s="84"/>
-      <c r="Q67" s="84"/>
-      <c r="R67" s="84"/>
-      <c r="S67" s="84"/>
-      <c r="T67" s="84"/>
-      <c r="U67" s="85"/>
-      <c r="Y67" s="93"/>
-      <c r="Z67" s="93"/>
-      <c r="AA67" s="93"/>
-      <c r="AB67" s="93"/>
-      <c r="AC67" s="93"/>
-      <c r="AD67" s="93"/>
-      <c r="AE67" s="93"/>
-      <c r="AF67" s="93"/>
+      <c r="K67" s="80"/>
+      <c r="L67" s="80"/>
+      <c r="M67" s="80"/>
+      <c r="N67" s="80"/>
+      <c r="O67" s="80"/>
+      <c r="P67" s="80"/>
+      <c r="Q67" s="80"/>
+      <c r="R67" s="80"/>
+      <c r="S67" s="80"/>
+      <c r="T67" s="80"/>
+      <c r="U67" s="81"/>
+      <c r="Y67" s="137"/>
+      <c r="Z67" s="137"/>
+      <c r="AA67" s="137"/>
+      <c r="AB67" s="137"/>
+      <c r="AC67" s="137"/>
+      <c r="AD67" s="137"/>
+      <c r="AE67" s="137"/>
+      <c r="AF67" s="137"/>
     </row>
     <row r="68" spans="2:32" ht="30" x14ac:dyDescent="0.6">
       <c r="C68" s="2"/>
@@ -3442,121 +3506,121 @@
       <c r="AF69" s="30"/>
     </row>
     <row r="70" spans="2:32" s="36" customFormat="1" ht="83.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="C70" s="76" t="s">
-        <v>47</v>
-      </c>
-      <c r="D70" s="76"/>
-      <c r="E70" s="76"/>
-      <c r="F70" s="76"/>
-      <c r="G70" s="76"/>
-      <c r="H70" s="76"/>
-      <c r="I70" s="76"/>
-      <c r="J70" s="76"/>
-      <c r="K70" s="76"/>
-      <c r="L70" s="76"/>
-      <c r="M70" s="76"/>
-      <c r="N70" s="76"/>
-      <c r="O70" s="76"/>
-      <c r="P70" s="76"/>
-      <c r="Q70" s="76"/>
-      <c r="R70" s="76"/>
-      <c r="S70" s="76"/>
-      <c r="T70" s="76"/>
-      <c r="U70" s="76"/>
+      <c r="C70" s="152" t="s">
+        <v>44</v>
+      </c>
+      <c r="D70" s="152"/>
+      <c r="E70" s="152"/>
+      <c r="F70" s="152"/>
+      <c r="G70" s="152"/>
+      <c r="H70" s="152"/>
+      <c r="I70" s="152"/>
+      <c r="J70" s="152"/>
+      <c r="K70" s="152"/>
+      <c r="L70" s="152"/>
+      <c r="M70" s="152"/>
+      <c r="N70" s="152"/>
+      <c r="O70" s="152"/>
+      <c r="P70" s="152"/>
+      <c r="Q70" s="152"/>
+      <c r="R70" s="152"/>
+      <c r="S70" s="152"/>
+      <c r="T70" s="152"/>
+      <c r="U70" s="152"/>
     </row>
     <row r="71" spans="2:32" s="36" customFormat="1" ht="83.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="B71" s="77" t="s">
-        <v>54</v>
-      </c>
-      <c r="C71" s="77"/>
-      <c r="D71" s="77"/>
-      <c r="E71" s="77"/>
-      <c r="F71" s="77"/>
-      <c r="G71" s="77"/>
-      <c r="H71" s="77"/>
-      <c r="I71" s="77"/>
-      <c r="J71" s="77"/>
-      <c r="K71" s="77"/>
-      <c r="L71" s="77"/>
-      <c r="M71" s="77"/>
-      <c r="N71" s="77"/>
-      <c r="O71" s="77"/>
-      <c r="P71" s="77"/>
-      <c r="Q71" s="77"/>
-      <c r="R71" s="77"/>
-      <c r="S71" s="77"/>
-      <c r="T71" s="77"/>
+      <c r="B71" s="153" t="s">
+        <v>51</v>
+      </c>
+      <c r="C71" s="153"/>
+      <c r="D71" s="153"/>
+      <c r="E71" s="153"/>
+      <c r="F71" s="153"/>
+      <c r="G71" s="153"/>
+      <c r="H71" s="153"/>
+      <c r="I71" s="153"/>
+      <c r="J71" s="153"/>
+      <c r="K71" s="153"/>
+      <c r="L71" s="153"/>
+      <c r="M71" s="153"/>
+      <c r="N71" s="153"/>
+      <c r="O71" s="153"/>
+      <c r="P71" s="153"/>
+      <c r="Q71" s="153"/>
+      <c r="R71" s="153"/>
+      <c r="S71" s="153"/>
+      <c r="T71" s="153"/>
       <c r="U71" s="63"/>
     </row>
     <row r="72" spans="2:32" s="36" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="C72" s="90" t="s">
-        <v>53</v>
-      </c>
-      <c r="D72" s="90"/>
-      <c r="E72" s="90"/>
-      <c r="F72" s="90"/>
-      <c r="G72" s="90"/>
-      <c r="H72" s="90"/>
-      <c r="I72" s="90"/>
-      <c r="J72" s="90"/>
-      <c r="K72" s="90"/>
-      <c r="L72" s="90"/>
-      <c r="M72" s="90"/>
-      <c r="N72" s="90"/>
-      <c r="O72" s="90"/>
-      <c r="P72" s="90"/>
-      <c r="Q72" s="90"/>
-      <c r="R72" s="90"/>
-      <c r="S72" s="90"/>
-      <c r="T72" s="90"/>
-      <c r="U72" s="90"/>
-      <c r="V72" s="90"/>
+      <c r="C72" s="159" t="s">
+        <v>50</v>
+      </c>
+      <c r="D72" s="159"/>
+      <c r="E72" s="159"/>
+      <c r="F72" s="159"/>
+      <c r="G72" s="159"/>
+      <c r="H72" s="159"/>
+      <c r="I72" s="159"/>
+      <c r="J72" s="159"/>
+      <c r="K72" s="159"/>
+      <c r="L72" s="159"/>
+      <c r="M72" s="159"/>
+      <c r="N72" s="159"/>
+      <c r="O72" s="159"/>
+      <c r="P72" s="159"/>
+      <c r="Q72" s="159"/>
+      <c r="R72" s="159"/>
+      <c r="S72" s="159"/>
+      <c r="T72" s="159"/>
+      <c r="U72" s="159"/>
+      <c r="V72" s="159"/>
     </row>
     <row r="73" spans="2:32" s="36" customFormat="1" ht="60.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="C73" s="82" t="s">
-        <v>48</v>
-      </c>
-      <c r="D73" s="82"/>
-      <c r="E73" s="82"/>
-      <c r="F73" s="82"/>
-      <c r="G73" s="82"/>
-      <c r="H73" s="82"/>
-      <c r="I73" s="82"/>
-      <c r="J73" s="82"/>
-      <c r="K73" s="82"/>
-      <c r="L73" s="82"/>
-      <c r="M73" s="82"/>
-      <c r="N73" s="82"/>
-      <c r="O73" s="82"/>
-      <c r="P73" s="82"/>
-      <c r="Q73" s="82"/>
-      <c r="R73" s="82"/>
-      <c r="S73" s="82"/>
-      <c r="T73" s="82"/>
-      <c r="U73" s="82"/>
+      <c r="C73" s="156" t="s">
+        <v>45</v>
+      </c>
+      <c r="D73" s="156"/>
+      <c r="E73" s="156"/>
+      <c r="F73" s="156"/>
+      <c r="G73" s="156"/>
+      <c r="H73" s="156"/>
+      <c r="I73" s="156"/>
+      <c r="J73" s="156"/>
+      <c r="K73" s="156"/>
+      <c r="L73" s="156"/>
+      <c r="M73" s="156"/>
+      <c r="N73" s="156"/>
+      <c r="O73" s="156"/>
+      <c r="P73" s="156"/>
+      <c r="Q73" s="156"/>
+      <c r="R73" s="156"/>
+      <c r="S73" s="156"/>
+      <c r="T73" s="156"/>
+      <c r="U73" s="156"/>
     </row>
     <row r="74" spans="2:32" s="36" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="C74" s="82" t="s">
-        <v>49</v>
-      </c>
-      <c r="D74" s="82"/>
-      <c r="E74" s="82"/>
-      <c r="F74" s="82"/>
-      <c r="G74" s="82"/>
-      <c r="H74" s="82"/>
-      <c r="I74" s="82"/>
-      <c r="J74" s="82"/>
-      <c r="K74" s="82"/>
-      <c r="L74" s="82"/>
-      <c r="M74" s="82"/>
-      <c r="N74" s="82"/>
-      <c r="O74" s="82"/>
-      <c r="P74" s="82"/>
-      <c r="Q74" s="82"/>
-      <c r="R74" s="82"/>
-      <c r="S74" s="82"/>
-      <c r="T74" s="82"/>
-      <c r="U74" s="82"/>
+      <c r="C74" s="156" t="s">
+        <v>46</v>
+      </c>
+      <c r="D74" s="156"/>
+      <c r="E74" s="156"/>
+      <c r="F74" s="156"/>
+      <c r="G74" s="156"/>
+      <c r="H74" s="156"/>
+      <c r="I74" s="156"/>
+      <c r="J74" s="156"/>
+      <c r="K74" s="156"/>
+      <c r="L74" s="156"/>
+      <c r="M74" s="156"/>
+      <c r="N74" s="156"/>
+      <c r="O74" s="156"/>
+      <c r="P74" s="156"/>
+      <c r="Q74" s="156"/>
+      <c r="R74" s="156"/>
+      <c r="S74" s="156"/>
+      <c r="T74" s="156"/>
+      <c r="U74" s="156"/>
     </row>
     <row r="75" spans="2:32" s="36" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.65">
       <c r="C75" s="46"/>
@@ -3581,71 +3645,71 @@
       <c r="V75" s="46"/>
     </row>
     <row r="76" spans="2:32" s="36" customFormat="1" ht="172.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="C76" s="83" t="s">
-        <v>55</v>
-      </c>
-      <c r="D76" s="83"/>
-      <c r="E76" s="83"/>
-      <c r="F76" s="83"/>
-      <c r="G76" s="83"/>
-      <c r="H76" s="83"/>
-      <c r="I76" s="83"/>
-      <c r="J76" s="83"/>
-      <c r="K76" s="83"/>
-      <c r="L76" s="83"/>
-      <c r="M76" s="83"/>
-      <c r="N76" s="83"/>
-      <c r="O76" s="83"/>
-      <c r="P76" s="83"/>
-      <c r="Q76" s="83"/>
-      <c r="R76" s="83"/>
-      <c r="S76" s="83"/>
-      <c r="T76" s="83"/>
-      <c r="U76" s="83"/>
+      <c r="C76" s="157" t="s">
+        <v>52</v>
+      </c>
+      <c r="D76" s="157"/>
+      <c r="E76" s="157"/>
+      <c r="F76" s="157"/>
+      <c r="G76" s="157"/>
+      <c r="H76" s="157"/>
+      <c r="I76" s="157"/>
+      <c r="J76" s="157"/>
+      <c r="K76" s="157"/>
+      <c r="L76" s="157"/>
+      <c r="M76" s="157"/>
+      <c r="N76" s="157"/>
+      <c r="O76" s="157"/>
+      <c r="P76" s="157"/>
+      <c r="Q76" s="157"/>
+      <c r="R76" s="157"/>
+      <c r="S76" s="157"/>
+      <c r="T76" s="157"/>
+      <c r="U76" s="157"/>
     </row>
     <row r="77" spans="2:32" s="36" customFormat="1" ht="11.5" hidden="1" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="C77" s="91"/>
-      <c r="D77" s="91"/>
-      <c r="E77" s="91"/>
-      <c r="F77" s="91"/>
-      <c r="G77" s="91"/>
-      <c r="H77" s="91"/>
-      <c r="I77" s="91"/>
-      <c r="J77" s="91"/>
-      <c r="K77" s="91"/>
-      <c r="L77" s="91"/>
-      <c r="M77" s="91"/>
-      <c r="N77" s="91"/>
-      <c r="O77" s="91"/>
-      <c r="P77" s="91"/>
-      <c r="Q77" s="91"/>
-      <c r="R77" s="91"/>
-      <c r="S77" s="91"/>
-      <c r="T77" s="91"/>
-      <c r="U77" s="91"/>
+      <c r="C77" s="135"/>
+      <c r="D77" s="135"/>
+      <c r="E77" s="135"/>
+      <c r="F77" s="135"/>
+      <c r="G77" s="135"/>
+      <c r="H77" s="135"/>
+      <c r="I77" s="135"/>
+      <c r="J77" s="135"/>
+      <c r="K77" s="135"/>
+      <c r="L77" s="135"/>
+      <c r="M77" s="135"/>
+      <c r="N77" s="135"/>
+      <c r="O77" s="135"/>
+      <c r="P77" s="135"/>
+      <c r="Q77" s="135"/>
+      <c r="R77" s="135"/>
+      <c r="S77" s="135"/>
+      <c r="T77" s="135"/>
+      <c r="U77" s="135"/>
     </row>
     <row r="78" spans="2:32" ht="25.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C78" s="74" t="s">
-        <v>38</v>
-      </c>
-      <c r="D78" s="74"/>
-      <c r="E78" s="74"/>
-      <c r="F78" s="74"/>
-      <c r="G78" s="74"/>
-      <c r="H78" s="74"/>
-      <c r="I78" s="74"/>
-      <c r="J78" s="74"/>
-      <c r="K78" s="74"/>
-      <c r="L78" s="74"/>
-      <c r="M78" s="74"/>
-      <c r="N78" s="74"/>
-      <c r="O78" s="74"/>
-      <c r="P78" s="74"/>
-      <c r="Q78" s="74"/>
-      <c r="R78" s="74"/>
-      <c r="S78" s="74"/>
-      <c r="T78" s="74"/>
-      <c r="U78" s="74"/>
+      <c r="C78" s="150" t="s">
+        <v>35</v>
+      </c>
+      <c r="D78" s="150"/>
+      <c r="E78" s="150"/>
+      <c r="F78" s="150"/>
+      <c r="G78" s="150"/>
+      <c r="H78" s="150"/>
+      <c r="I78" s="150"/>
+      <c r="J78" s="150"/>
+      <c r="K78" s="150"/>
+      <c r="L78" s="150"/>
+      <c r="M78" s="150"/>
+      <c r="N78" s="150"/>
+      <c r="O78" s="150"/>
+      <c r="P78" s="150"/>
+      <c r="Q78" s="150"/>
+      <c r="R78" s="150"/>
+      <c r="S78" s="150"/>
+      <c r="T78" s="150"/>
+      <c r="U78" s="150"/>
     </row>
     <row r="79" spans="2:32" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.6">
       <c r="C79" s="14"/>
@@ -3808,22 +3872,22 @@
       <c r="G86" s="117"/>
       <c r="H86" s="117"/>
       <c r="I86" s="117"/>
-      <c r="J86" s="102"/>
-      <c r="K86" s="102"/>
-      <c r="L86" s="102"/>
-      <c r="M86" s="102"/>
-      <c r="N86" s="102"/>
-      <c r="O86" s="102"/>
-      <c r="P86" s="102"/>
-      <c r="Q86" s="102"/>
-      <c r="R86" s="102"/>
-      <c r="S86" s="102"/>
+      <c r="J86" s="115"/>
+      <c r="K86" s="115"/>
+      <c r="L86" s="115"/>
+      <c r="M86" s="115"/>
+      <c r="N86" s="115"/>
+      <c r="O86" s="115"/>
+      <c r="P86" s="115"/>
+      <c r="Q86" s="115"/>
+      <c r="R86" s="115"/>
+      <c r="S86" s="115"/>
       <c r="T86" s="35"/>
       <c r="U86" s="2"/>
     </row>
     <row r="87" spans="2:22" ht="31" x14ac:dyDescent="0.6">
       <c r="C87" s="118" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D87" s="118"/>
       <c r="E87" s="118"/>
@@ -3845,7 +3909,7 @@
     </row>
     <row r="88" spans="2:22" ht="71" customHeight="1" x14ac:dyDescent="0.6">
       <c r="C88" s="66" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D88" s="59"/>
       <c r="E88" s="59"/>
@@ -3892,25 +3956,25 @@
     </row>
     <row r="90" spans="2:22" ht="243.5" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="93" spans="2:22" x14ac:dyDescent="0.55000000000000004">
-      <c r="C93" s="80"/>
-      <c r="D93" s="80"/>
-      <c r="E93" s="80"/>
-      <c r="F93" s="80"/>
-      <c r="G93" s="80"/>
-      <c r="H93" s="80"/>
-      <c r="I93" s="80"/>
-      <c r="J93" s="80"/>
-      <c r="K93" s="80"/>
-      <c r="L93" s="80"/>
-      <c r="M93" s="80"/>
-      <c r="N93" s="80"/>
-      <c r="O93" s="80"/>
-      <c r="P93" s="80"/>
-      <c r="Q93" s="80"/>
-      <c r="R93" s="80"/>
-      <c r="S93" s="80"/>
-      <c r="T93" s="80"/>
-      <c r="U93" s="80"/>
+      <c r="C93" s="114"/>
+      <c r="D93" s="114"/>
+      <c r="E93" s="114"/>
+      <c r="F93" s="114"/>
+      <c r="G93" s="114"/>
+      <c r="H93" s="114"/>
+      <c r="I93" s="114"/>
+      <c r="J93" s="114"/>
+      <c r="K93" s="114"/>
+      <c r="L93" s="114"/>
+      <c r="M93" s="114"/>
+      <c r="N93" s="114"/>
+      <c r="O93" s="114"/>
+      <c r="P93" s="114"/>
+      <c r="Q93" s="114"/>
+      <c r="R93" s="114"/>
+      <c r="S93" s="114"/>
+      <c r="T93" s="114"/>
+      <c r="U93" s="114"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -3920,37 +3984,21 @@
     </dataRefs>
   </dataConsolidate>
   <mergeCells count="77">
-    <mergeCell ref="AA53:AC53"/>
-    <mergeCell ref="M62:U62"/>
-    <mergeCell ref="J62:L62"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="C47:U47"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="N14:U14"/>
-    <mergeCell ref="C18:J18"/>
-    <mergeCell ref="C44:U46"/>
-    <mergeCell ref="C22:J22"/>
-    <mergeCell ref="K22:U22"/>
-    <mergeCell ref="K18:U18"/>
-    <mergeCell ref="K20:U20"/>
-    <mergeCell ref="K23:S23"/>
-    <mergeCell ref="C25:U25"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C55:P55"/>
-    <mergeCell ref="C53:U53"/>
-    <mergeCell ref="C52:U52"/>
-    <mergeCell ref="C48:V48"/>
-    <mergeCell ref="C43:U43"/>
-    <mergeCell ref="C33:U33"/>
-    <mergeCell ref="C93:U93"/>
-    <mergeCell ref="J86:S86"/>
-    <mergeCell ref="S83:T83"/>
-    <mergeCell ref="E86:I86"/>
-    <mergeCell ref="C87:T87"/>
-    <mergeCell ref="C83:R83"/>
-    <mergeCell ref="C84:P84"/>
-    <mergeCell ref="C89:U89"/>
+    <mergeCell ref="L62:U62"/>
+    <mergeCell ref="C78:U78"/>
+    <mergeCell ref="C27:U27"/>
+    <mergeCell ref="C70:U70"/>
+    <mergeCell ref="B71:T71"/>
+    <mergeCell ref="C42:U42"/>
+    <mergeCell ref="C54:Q54"/>
+    <mergeCell ref="K37:U37"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="C73:U73"/>
+    <mergeCell ref="C74:U74"/>
+    <mergeCell ref="C76:U76"/>
+    <mergeCell ref="C34:P34"/>
+    <mergeCell ref="C31:U31"/>
+    <mergeCell ref="C72:V72"/>
     <mergeCell ref="C6:U6"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="E32:I32"/>
@@ -3967,39 +4015,55 @@
     <mergeCell ref="C20:J20"/>
     <mergeCell ref="I14:J14"/>
     <mergeCell ref="I15:J15"/>
+    <mergeCell ref="C52:U52"/>
+    <mergeCell ref="C48:V48"/>
+    <mergeCell ref="C43:U43"/>
+    <mergeCell ref="C33:U33"/>
+    <mergeCell ref="C93:U93"/>
+    <mergeCell ref="J86:S86"/>
+    <mergeCell ref="S83:T83"/>
+    <mergeCell ref="E86:I86"/>
+    <mergeCell ref="C87:T87"/>
+    <mergeCell ref="C83:R83"/>
+    <mergeCell ref="C84:P84"/>
+    <mergeCell ref="C89:U89"/>
     <mergeCell ref="C77:U77"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="J59:K59"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="C47:U47"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="N14:U14"/>
+    <mergeCell ref="C18:J18"/>
+    <mergeCell ref="C44:U46"/>
+    <mergeCell ref="C22:J22"/>
+    <mergeCell ref="K22:U22"/>
+    <mergeCell ref="K18:U18"/>
+    <mergeCell ref="K20:U20"/>
+    <mergeCell ref="K23:S23"/>
+    <mergeCell ref="C25:U25"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="J65:U65"/>
+    <mergeCell ref="C65:I65"/>
+    <mergeCell ref="J67:U67"/>
+    <mergeCell ref="C67:I67"/>
+    <mergeCell ref="AA53:AC53"/>
+    <mergeCell ref="C55:P55"/>
+    <mergeCell ref="C53:U53"/>
     <mergeCell ref="AA58:AC58"/>
     <mergeCell ref="Y67:AF67"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="K65:U65"/>
-    <mergeCell ref="C65:J65"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="J59:K59"/>
     <mergeCell ref="L58:O58"/>
     <mergeCell ref="L59:O59"/>
     <mergeCell ref="C62:I62"/>
     <mergeCell ref="Y59:AA59"/>
     <mergeCell ref="P58:U58"/>
     <mergeCell ref="P59:U59"/>
-    <mergeCell ref="C78:U78"/>
-    <mergeCell ref="C27:U27"/>
-    <mergeCell ref="C70:U70"/>
-    <mergeCell ref="B71:T71"/>
-    <mergeCell ref="C42:U42"/>
-    <mergeCell ref="C54:Q54"/>
-    <mergeCell ref="K37:U37"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="C73:U73"/>
-    <mergeCell ref="C74:U74"/>
-    <mergeCell ref="C76:U76"/>
-    <mergeCell ref="K67:U67"/>
-    <mergeCell ref="C34:P34"/>
-    <mergeCell ref="C31:U31"/>
-    <mergeCell ref="C67:J67"/>
-    <mergeCell ref="C72:V72"/>
+    <mergeCell ref="J62:K62"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="129" scale="76" firstPageNumber="0" fitToHeight="0" orientation="portrait" errors="blank" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
+  <pageSetup paperSize="209" scale="26" firstPageNumber="0" fitToHeight="0" orientation="portrait" errors="blank" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>